<commit_message>
print the command of missing resuts
</commit_message>
<xml_diff>
--- a/scripts.xlsx
+++ b/scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\01.Code\FedProC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B98949-40CA-4E34-A9B3-85182F405099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6338E4C9-ED0E-4335-A7A5-692BC7A852E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4676614C-C8DD-4D38-BD66-2E739B6203C6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="24">
   <si>
     <t>MSE</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>CryptoDataDownloadDay</t>
+  </si>
+  <si>
+    <t>script</t>
   </si>
 </sst>
 </file>
@@ -486,8 +489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF8F8CC3-6A9E-45FD-B534-488B8E56A491}">
   <dimension ref="A1:N84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +543,9 @@
       <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>

</xml_diff>